<commit_message>
Changes default of capital replacement rate to True.
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-synfuels-from-FT-from-wood-gasification-with-CCS.xlsx
+++ b/premise/data/additional_inventories/lci-synfuels-from-FT-from-wood-gasification-with-CCS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/Github/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FCD280B-775D-FB49-A686-B7823C2343CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A892DB-E724-6747-9AB7-F17D2BEF30AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35440" yWindow="280" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12260" yWindow="1900" windowWidth="44800" windowHeight="23000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FT fuel - Diesel" sheetId="1" r:id="rId1"/>
@@ -304,11 +304,6 @@
     <t>Carbon dioxide, in air</t>
   </si>
   <si>
-    <t>Adapted from van der Giesen et al. 2014. Density of syngas: 0.470kg/m3 @1 bar. LHV: 23.9 MJ/kg.
-The source for CO2 is from the gasification step to produce the H2. Hence, it comes free of burden.
-The CO2, instead of being stored underground, is embodied in teh fuel, hence no correction is needed.</t>
-  </si>
-  <si>
     <t>hydrogen, gaseous, 25 bar</t>
   </si>
   <si>
@@ -364,6 +359,9 @@
   </si>
   <si>
     <t>liquefied petroleum gas production, synthetic, Fischer Tropsch process, hydrogen from wood gasification, energy allocation, with carbon capture and storage</t>
+  </si>
+  <si>
+    <t>Adapted from van der Giesen et al. 2014. Density of syngas: 0.470kg/m3 @1 bar. LHV: 23.9 MJ/kg. The source for CO2 is from the gasification step to produce the H2. Hence, it comes free of burden. The CO2, instead of being stored underground, is embodied in the fuel, hence no correction is needed.</t>
   </si>
 </sst>
 </file>
@@ -783,8 +781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K596"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A144" workbookViewId="0">
-      <selection activeCell="B163" sqref="B163"/>
+    <sheetView tabSelected="1" topLeftCell="A208" workbookViewId="0">
+      <selection activeCell="G262" sqref="G262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1294,7 +1292,7 @@
         <v>18</v>
       </c>
       <c r="K34" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -2008,7 +2006,7 @@
         <v>18</v>
       </c>
       <c r="K78" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="79" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -2239,7 +2237,7 @@
         <v>0</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="92" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -2334,7 +2332,7 @@
     </row>
     <row r="101" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A101" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B101" s="8">
         <v>1</v>
@@ -2493,7 +2491,7 @@
         <v>0</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="110" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -2509,7 +2507,7 @@
         <v>2</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="112" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -2588,7 +2586,7 @@
     </row>
     <row r="119" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A119" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B119" s="8">
         <v>1</v>
@@ -2603,7 +2601,7 @@
         <v>15</v>
       </c>
       <c r="G119" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H119" s="8" t="s">
         <v>36</v>
@@ -2626,7 +2624,7 @@
         <v>18</v>
       </c>
       <c r="G120" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H120" s="8" t="s">
         <v>36</v>
@@ -2744,7 +2742,7 @@
         <v>0</v>
       </c>
       <c r="B127" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="128" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -2760,7 +2758,7 @@
         <v>2</v>
       </c>
       <c r="B129" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="130" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -2839,7 +2837,7 @@
     </row>
     <row r="137" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A137" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B137" s="8">
         <v>1</v>
@@ -2854,7 +2852,7 @@
         <v>15</v>
       </c>
       <c r="G137" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H137" s="8" t="s">
         <v>36</v>
@@ -2865,7 +2863,7 @@
     </row>
     <row r="138" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A138" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B138" s="8">
         <v>0.98</v>
@@ -2880,7 +2878,7 @@
         <v>18</v>
       </c>
       <c r="G138" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H138" s="8" t="s">
         <v>36</v>
@@ -2998,7 +2996,7 @@
         <v>0</v>
       </c>
       <c r="B145" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="146" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -3014,7 +3012,7 @@
         <v>2</v>
       </c>
       <c r="B147" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="148" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -3093,7 +3091,7 @@
     </row>
     <row r="155" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A155" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B155" s="8">
         <v>1</v>
@@ -3108,7 +3106,7 @@
         <v>15</v>
       </c>
       <c r="G155" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H155" s="8" t="s">
         <v>36</v>
@@ -3119,7 +3117,7 @@
     </row>
     <row r="156" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A156" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B156" s="8">
         <v>2.1</v>
@@ -3134,7 +3132,7 @@
         <v>18</v>
       </c>
       <c r="G156" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H156" s="8" t="s">
         <v>36</v>
@@ -3254,7 +3252,7 @@
         <v>0</v>
       </c>
       <c r="B163" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="164" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -3349,7 +3347,7 @@
     </row>
     <row r="173" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A173" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B173" s="8">
         <v>1</v>
@@ -3375,7 +3373,7 @@
     </row>
     <row r="174" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A174" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B174" s="8">
         <v>2.35</v>
@@ -3390,7 +3388,7 @@
         <v>18</v>
       </c>
       <c r="G174" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H174" s="8" t="s">
         <v>36</v>
@@ -3508,7 +3506,7 @@
         <v>0</v>
       </c>
       <c r="B181" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="182" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -3524,7 +3522,7 @@
         <v>2</v>
       </c>
       <c r="B183" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="184" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -3603,7 +3601,7 @@
     </row>
     <row r="191" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A191" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B191" s="8">
         <v>1</v>
@@ -3618,7 +3616,7 @@
         <v>15</v>
       </c>
       <c r="G191" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H191" s="8" t="s">
         <v>36</v>
@@ -3626,7 +3624,7 @@
     </row>
     <row r="192" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A192" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B192" s="8">
         <v>2.3199999999999998</v>
@@ -3641,7 +3639,7 @@
         <v>18</v>
       </c>
       <c r="G192" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H192" s="8" t="s">
         <v>36</v>
@@ -3759,7 +3757,7 @@
         <v>0</v>
       </c>
       <c r="B199" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="200" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -3775,7 +3773,7 @@
         <v>2</v>
       </c>
       <c r="B201" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="202" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -3854,7 +3852,7 @@
     </row>
     <row r="209" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A209" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B209" s="8">
         <v>1</v>
@@ -3869,7 +3867,7 @@
         <v>15</v>
       </c>
       <c r="G209" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H209" s="8" t="s">
         <v>36</v>
@@ -3880,7 +3878,7 @@
     </row>
     <row r="210" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A210" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B210" s="8">
         <v>2.2599999999999998</v>
@@ -3895,7 +3893,7 @@
         <v>18</v>
       </c>
       <c r="G210" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H210" s="8" t="s">
         <v>36</v>
@@ -4013,7 +4011,7 @@
         <v>0</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.2">
@@ -4029,7 +4027,7 @@
         <v>2</v>
       </c>
       <c r="B219" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.2">
@@ -4061,7 +4059,7 @@
         <v>9</v>
       </c>
       <c r="B223" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.2">
@@ -4069,7 +4067,7 @@
         <v>34</v>
       </c>
       <c r="B224" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="225" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4130,7 +4128,7 @@
     </row>
     <row r="228" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B228">
         <v>2.2799999999999998</v>
@@ -4145,7 +4143,7 @@
         <v>18</v>
       </c>
       <c r="G228" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="229" spans="1:8" x14ac:dyDescent="0.2">
@@ -4247,7 +4245,7 @@
         <v>0</v>
       </c>
       <c r="B235" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="236" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -4263,7 +4261,7 @@
         <v>2</v>
       </c>
       <c r="B237" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="238" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -4336,7 +4334,7 @@
     </row>
     <row r="245" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A245" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B245" s="8">
         <v>0.875</v>
@@ -4351,7 +4349,7 @@
         <v>18</v>
       </c>
       <c r="G245" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="246" spans="1:7" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -4371,7 +4369,7 @@
         <v>18</v>
       </c>
       <c r="G246" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="247" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -4457,7 +4455,7 @@
         <v>0</v>
       </c>
       <c r="B252" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="253" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -4473,7 +4471,7 @@
         <v>2</v>
       </c>
       <c r="B254" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="255" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -4505,7 +4503,7 @@
         <v>9</v>
       </c>
       <c r="B258" s="8" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
     </row>
     <row r="259" spans="1:7" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -4538,7 +4536,7 @@
     </row>
     <row r="261" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A261" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B261" s="8">
         <v>1</v>
@@ -4553,7 +4551,7 @@
         <v>15</v>
       </c>
       <c r="G261" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="262" spans="1:7" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -4573,7 +4571,7 @@
         <v>18</v>
       </c>
       <c r="G262" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="263" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>